<commit_message>
mobile_upload && fixed employee_kpi.present_file
</commit_message>
<xml_diff>
--- a/app/2.xlsx
+++ b/app/2.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22206"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5CA6A0B7-BC45-4463-8F8F-ADEFCC2864C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Flask\hrci_back\app\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA03FF8-E3BC-41D6-B53C-F001880E3EC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,11 +37,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -65,7 +70,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -379,13 +384,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A192" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B213"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="M101" sqref="M101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>62000</v>
       </c>
@@ -402,7 +407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>62001</v>
       </c>
@@ -410,7 +415,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>62002</v>
       </c>
@@ -418,7 +423,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>62003</v>
       </c>
@@ -426,7 +431,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>62004</v>
       </c>
@@ -434,7 +439,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>62005</v>
       </c>
@@ -442,7 +447,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>62006</v>
       </c>
@@ -450,7 +455,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>62007</v>
       </c>
@@ -458,7 +463,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>62008</v>
       </c>
@@ -466,7 +471,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>62009</v>
       </c>
@@ -474,7 +479,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>62010</v>
       </c>
@@ -482,7 +487,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>62011</v>
       </c>
@@ -490,7 +495,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>62012</v>
       </c>
@@ -498,7 +503,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>62013</v>
       </c>
@@ -506,7 +511,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>62014</v>
       </c>
@@ -514,7 +519,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>62015</v>
       </c>
@@ -522,7 +527,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>62016</v>
       </c>
@@ -530,7 +535,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>62017</v>
       </c>
@@ -538,7 +543,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>62018</v>
       </c>
@@ -546,7 +551,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>62019</v>
       </c>
@@ -554,7 +559,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>62020</v>
       </c>
@@ -562,7 +567,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>62021</v>
       </c>
@@ -570,7 +575,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>62022</v>
       </c>
@@ -578,7 +583,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>62023</v>
       </c>
@@ -586,7 +591,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>62024</v>
       </c>
@@ -594,7 +599,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>62025</v>
       </c>
@@ -602,7 +607,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>62026</v>
       </c>
@@ -610,7 +615,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>62027</v>
       </c>
@@ -618,7 +623,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>62028</v>
       </c>
@@ -626,7 +631,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>62029</v>
       </c>
@@ -634,7 +639,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>62030</v>
       </c>
@@ -642,7 +647,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>62031</v>
       </c>
@@ -650,7 +655,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>62032</v>
       </c>
@@ -658,7 +663,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>62033</v>
       </c>
@@ -666,7 +671,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>62034</v>
       </c>
@@ -674,7 +679,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>62035</v>
       </c>
@@ -682,7 +687,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>62036</v>
       </c>
@@ -690,7 +695,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>62037</v>
       </c>
@@ -698,7 +703,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>62038</v>
       </c>
@@ -706,7 +711,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>62039</v>
       </c>
@@ -714,7 +719,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>62040</v>
       </c>
@@ -722,7 +727,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>62041</v>
       </c>
@@ -730,7 +735,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>62042</v>
       </c>
@@ -738,7 +743,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>62043</v>
       </c>
@@ -746,7 +751,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>62044</v>
       </c>
@@ -754,7 +759,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>62045</v>
       </c>
@@ -762,7 +767,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>62046</v>
       </c>
@@ -770,7 +775,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>62047</v>
       </c>
@@ -778,7 +783,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>62048</v>
       </c>
@@ -786,7 +791,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>62049</v>
       </c>
@@ -794,7 +799,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>62050</v>
       </c>
@@ -802,7 +807,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>62051</v>
       </c>
@@ -810,7 +815,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>62052</v>
       </c>
@@ -818,7 +823,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>62053</v>
       </c>
@@ -826,7 +831,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>62054</v>
       </c>
@@ -834,7 +839,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>62055</v>
       </c>
@@ -842,7 +847,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>62056</v>
       </c>
@@ -850,7 +855,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>62057</v>
       </c>
@@ -858,7 +863,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>62058</v>
       </c>
@@ -866,7 +871,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>62059</v>
       </c>
@@ -874,7 +879,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>62060</v>
       </c>
@@ -882,7 +887,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>62061</v>
       </c>
@@ -890,7 +895,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62062</v>
       </c>
@@ -898,7 +903,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62063</v>
       </c>
@@ -906,7 +911,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>62064</v>
       </c>
@@ -914,7 +919,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>62065</v>
       </c>
@@ -922,7 +927,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>62066</v>
       </c>
@@ -930,7 +935,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>62067</v>
       </c>
@@ -938,7 +943,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>62068</v>
       </c>
@@ -946,7 +951,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>62069</v>
       </c>
@@ -954,7 +959,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>62070</v>
       </c>
@@ -962,7 +967,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>62071</v>
       </c>
@@ -970,7 +975,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>62072</v>
       </c>
@@ -978,7 +983,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>62073</v>
       </c>
@@ -986,7 +991,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>62074</v>
       </c>
@@ -994,7 +999,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>62075</v>
       </c>
@@ -1002,7 +1007,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>62076</v>
       </c>
@@ -1010,7 +1015,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>62077</v>
       </c>
@@ -1018,7 +1023,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>62078</v>
       </c>
@@ -1026,7 +1031,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>62079</v>
       </c>
@@ -1034,7 +1039,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>62080</v>
       </c>
@@ -1042,7 +1047,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>62081</v>
       </c>
@@ -1050,7 +1055,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>62082</v>
       </c>
@@ -1058,7 +1063,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>62083</v>
       </c>
@@ -1066,7 +1071,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>62084</v>
       </c>
@@ -1074,7 +1079,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>62085</v>
       </c>
@@ -1082,7 +1087,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>62086</v>
       </c>
@@ -1090,7 +1095,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>62087</v>
       </c>
@@ -1098,7 +1103,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>62088</v>
       </c>
@@ -1106,7 +1111,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>62089</v>
       </c>
@@ -1114,7 +1119,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>62090</v>
       </c>
@@ -1122,7 +1127,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>62091</v>
       </c>
@@ -1130,7 +1135,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>62092</v>
       </c>
@@ -1138,7 +1143,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>62093</v>
       </c>
@@ -1146,7 +1151,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>62094</v>
       </c>
@@ -1154,7 +1159,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>62095</v>
       </c>
@@ -1162,7 +1167,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>62096</v>
       </c>
@@ -1170,7 +1175,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>62097</v>
       </c>
@@ -1178,7 +1183,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>62098</v>
       </c>
@@ -1186,7 +1191,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>62099</v>
       </c>
@@ -1194,7 +1199,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>62100</v>
       </c>
@@ -1202,7 +1207,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>62101</v>
       </c>
@@ -1210,7 +1215,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>62102</v>
       </c>
@@ -1218,7 +1223,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>62103</v>
       </c>
@@ -1226,7 +1231,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>62104</v>
       </c>
@@ -1234,7 +1239,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>62105</v>
       </c>
@@ -1242,7 +1247,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>62106</v>
       </c>
@@ -1250,15 +1255,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
-      <c r="A108">
-        <v>62107</v>
-      </c>
-      <c r="B108">
-        <v>62107</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>62108</v>
       </c>
@@ -1266,7 +1263,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>62109</v>
       </c>
@@ -1274,7 +1271,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="111" spans="1:2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>62110</v>
       </c>
@@ -1282,7 +1279,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="112" spans="1:2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>62111</v>
       </c>
@@ -1290,7 +1287,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>62112</v>
       </c>
@@ -1298,7 +1295,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>62113</v>
       </c>
@@ -1306,7 +1303,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>62114</v>
       </c>
@@ -1314,7 +1311,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>62115</v>
       </c>
@@ -1322,7 +1319,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>62116</v>
       </c>
@@ -1330,7 +1327,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>62117</v>
       </c>
@@ -1338,7 +1335,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="119" spans="1:2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>62118</v>
       </c>
@@ -1346,7 +1343,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>62119</v>
       </c>
@@ -1354,7 +1351,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="121" spans="1:2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>62120</v>
       </c>
@@ -1362,7 +1359,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>62121</v>
       </c>
@@ -1370,7 +1367,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>62122</v>
       </c>
@@ -1378,7 +1375,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="124" spans="1:2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>62123</v>
       </c>
@@ -1386,7 +1383,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="125" spans="1:2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>62124</v>
       </c>
@@ -1394,7 +1391,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="126" spans="1:2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>62125</v>
       </c>
@@ -1402,7 +1399,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="127" spans="1:2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>62126</v>
       </c>
@@ -1410,7 +1407,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="128" spans="1:2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>62127</v>
       </c>
@@ -1418,7 +1415,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="129" spans="1:2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>62128</v>
       </c>
@@ -1426,7 +1423,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="130" spans="1:2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>62129</v>
       </c>
@@ -1434,7 +1431,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="131" spans="1:2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>62130</v>
       </c>
@@ -1442,7 +1439,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="132" spans="1:2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>62131</v>
       </c>
@@ -1450,7 +1447,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="133" spans="1:2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>62132</v>
       </c>
@@ -1458,7 +1455,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="134" spans="1:2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>62133</v>
       </c>
@@ -1466,7 +1463,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="135" spans="1:2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>62134</v>
       </c>
@@ -1474,7 +1471,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="136" spans="1:2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>62135</v>
       </c>
@@ -1482,7 +1479,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="137" spans="1:2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>62136</v>
       </c>
@@ -1490,7 +1487,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="138" spans="1:2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>62137</v>
       </c>
@@ -1498,7 +1495,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="139" spans="1:2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>62138</v>
       </c>
@@ -1506,7 +1503,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="140" spans="1:2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>62139</v>
       </c>
@@ -1514,7 +1511,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="141" spans="1:2">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>62140</v>
       </c>
@@ -1522,7 +1519,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="142" spans="1:2">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>62141</v>
       </c>
@@ -1530,7 +1527,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="143" spans="1:2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>62142</v>
       </c>
@@ -1538,7 +1535,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="144" spans="1:2">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>62143</v>
       </c>
@@ -1546,7 +1543,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="145" spans="1:2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>62144</v>
       </c>
@@ -1554,7 +1551,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="146" spans="1:2">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>62145</v>
       </c>
@@ -1562,7 +1559,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="147" spans="1:2">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>62146</v>
       </c>
@@ -1570,7 +1567,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="148" spans="1:2">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>62147</v>
       </c>
@@ -1578,7 +1575,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="149" spans="1:2">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>62148</v>
       </c>
@@ -1586,7 +1583,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="150" spans="1:2">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>62149</v>
       </c>
@@ -1594,7 +1591,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="151" spans="1:2">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>62150</v>
       </c>
@@ -1602,7 +1599,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="152" spans="1:2">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>62151</v>
       </c>
@@ -1610,7 +1607,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="153" spans="1:2">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>62152</v>
       </c>
@@ -1618,7 +1615,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="154" spans="1:2">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>62153</v>
       </c>
@@ -1626,7 +1623,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="155" spans="1:2">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>62154</v>
       </c>
@@ -1634,7 +1631,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="156" spans="1:2">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>62155</v>
       </c>
@@ -1642,7 +1639,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="157" spans="1:2">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>62156</v>
       </c>
@@ -1650,7 +1647,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="158" spans="1:2">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>62157</v>
       </c>
@@ -1658,7 +1655,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="159" spans="1:2">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>62158</v>
       </c>
@@ -1666,7 +1663,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="160" spans="1:2">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>62159</v>
       </c>
@@ -1674,7 +1671,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="161" spans="1:2">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>62160</v>
       </c>
@@ -1682,7 +1679,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="162" spans="1:2">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>62161</v>
       </c>
@@ -1690,7 +1687,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="163" spans="1:2">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>62162</v>
       </c>
@@ -1698,7 +1695,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="164" spans="1:2">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>62163</v>
       </c>
@@ -1706,7 +1703,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="165" spans="1:2">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>62164</v>
       </c>
@@ -1714,7 +1711,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="166" spans="1:2">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>62165</v>
       </c>
@@ -1722,7 +1719,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="167" spans="1:2">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>62166</v>
       </c>
@@ -1730,7 +1727,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="168" spans="1:2">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>62167</v>
       </c>
@@ -1738,7 +1735,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="169" spans="1:2">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>62168</v>
       </c>
@@ -1746,7 +1743,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="170" spans="1:2">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>62169</v>
       </c>
@@ -1754,7 +1751,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="171" spans="1:2">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>62170</v>
       </c>
@@ -1762,7 +1759,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="172" spans="1:2">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>62171</v>
       </c>
@@ -1770,7 +1767,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="173" spans="1:2">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>62172</v>
       </c>
@@ -1778,7 +1775,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="174" spans="1:2">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>62173</v>
       </c>
@@ -1786,7 +1783,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="175" spans="1:2">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>62174</v>
       </c>
@@ -1794,7 +1791,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="176" spans="1:2">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>62175</v>
       </c>
@@ -1802,7 +1799,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="177" spans="1:2">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>62176</v>
       </c>
@@ -1810,7 +1807,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="178" spans="1:2">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>62177</v>
       </c>
@@ -1818,7 +1815,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="179" spans="1:2">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>62178</v>
       </c>
@@ -1826,7 +1823,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="180" spans="1:2">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>62179</v>
       </c>
@@ -1834,7 +1831,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="181" spans="1:2">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>62180</v>
       </c>
@@ -1842,7 +1839,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="182" spans="1:2">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>62181</v>
       </c>
@@ -1850,7 +1847,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="183" spans="1:2">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>62182</v>
       </c>
@@ -1858,7 +1855,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="184" spans="1:2">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>62183</v>
       </c>
@@ -1866,7 +1863,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="185" spans="1:2">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>62184</v>
       </c>
@@ -1874,7 +1871,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="186" spans="1:2">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>62185</v>
       </c>
@@ -1882,7 +1879,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="187" spans="1:2">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>62186</v>
       </c>
@@ -1890,7 +1887,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="188" spans="1:2">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>62187</v>
       </c>
@@ -1898,7 +1895,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="189" spans="1:2">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>62188</v>
       </c>
@@ -1906,7 +1903,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="190" spans="1:2">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>62189</v>
       </c>
@@ -1914,7 +1911,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="191" spans="1:2">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>62190</v>
       </c>
@@ -1922,7 +1919,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="192" spans="1:2">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>62191</v>
       </c>
@@ -1930,7 +1927,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="193" spans="1:2">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>62192</v>
       </c>
@@ -1938,7 +1935,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="194" spans="1:2">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>62193</v>
       </c>
@@ -1946,7 +1943,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="195" spans="1:2">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>62194</v>
       </c>
@@ -1954,7 +1951,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="196" spans="1:2">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>62195</v>
       </c>
@@ -1962,7 +1959,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="197" spans="1:2">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>62196</v>
       </c>
@@ -1970,7 +1967,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="198" spans="1:2">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>62197</v>
       </c>
@@ -1978,7 +1975,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="199" spans="1:2">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>62198</v>
       </c>
@@ -1986,7 +1983,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="200" spans="1:2">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>62199</v>
       </c>
@@ -1994,7 +1991,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="201" spans="1:2">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>62200</v>
       </c>
@@ -2002,7 +1999,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="202" spans="1:2">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>62201</v>
       </c>
@@ -2010,7 +2007,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="203" spans="1:2">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>62202</v>
       </c>
@@ -2018,7 +2015,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="204" spans="1:2">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>62203</v>
       </c>
@@ -2026,7 +2023,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="205" spans="1:2">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>62204</v>
       </c>
@@ -2034,7 +2031,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="206" spans="1:2">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>62205</v>
       </c>
@@ -2042,7 +2039,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="207" spans="1:2">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>62206</v>
       </c>
@@ -2050,7 +2047,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="208" spans="1:2">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>62207</v>
       </c>
@@ -2058,7 +2055,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="209" spans="1:2">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>62208</v>
       </c>
@@ -2066,7 +2063,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="210" spans="1:2">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>62209</v>
       </c>
@@ -2074,7 +2071,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="211" spans="1:2">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>62210</v>
       </c>
@@ -2082,7 +2079,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="212" spans="1:2">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>62211</v>
       </c>
@@ -2090,7 +2087,7 @@
         <v>62107</v>
       </c>
     </row>
-    <row r="213" spans="1:2">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>62212</v>
       </c>

</xml_diff>